<commit_message>
New weapon creation algorithm
</commit_message>
<xml_diff>
--- a/Math/Weapon DPS.xlsx
+++ b/Math/Weapon DPS.xlsx
@@ -5,17 +5,18 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="188" firstSheet="0" activeTab="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="188" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
   <si>
     <t>Level</t>
   </si>
@@ -99,6 +100,66 @@
   </si>
   <si>
     <t>HP Gains</t>
+  </si>
+  <si>
+    <t>Weapon Level</t>
+  </si>
+  <si>
+    <t>Quality Multipliers:</t>
+  </si>
+  <si>
+    <t>Speed Brackets</t>
+  </si>
+  <si>
+    <t>Quality Mult</t>
+  </si>
+  <si>
+    <t>Quality</t>
+  </si>
+  <si>
+    <t>Mult</t>
+  </si>
+  <si>
+    <t>Bracket</t>
+  </si>
+  <si>
+    <t>Min Base</t>
+  </si>
+  <si>
+    <t>Max Base</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>Dreadful</t>
+  </si>
+  <si>
+    <t>Slow</t>
+  </si>
+  <si>
+    <t>Poor</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Per level increase</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Fast</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Great</t>
+  </si>
+  <si>
+    <t>Amazing</t>
   </si>
 </sst>
 </file>
@@ -106,29 +167,29 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
   <fonts count="4">
     <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -140,7 +201,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
@@ -149,43 +210,47 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellXfs count="2">
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -193,13 +258,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B33" activeCellId="0" pane="topLeft" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -211,7 +275,7 @@
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -219,7 +283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="C2" s="0" t="s">
         <v>1</v>
       </c>
@@ -245,7 +309,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
@@ -278,7 +342,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
@@ -311,7 +375,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
         <v>11</v>
       </c>
@@ -344,7 +408,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="7">
       <c r="C7" s="0" t="s">
         <v>1</v>
       </c>
@@ -370,7 +434,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
         <v>9</v>
       </c>
@@ -403,7 +467,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
         <v>10</v>
       </c>
@@ -436,7 +500,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
         <v>11</v>
       </c>
@@ -469,7 +533,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
         <v>12</v>
       </c>
@@ -495,7 +559,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
         <v>20</v>
       </c>
@@ -508,7 +572,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
         <v>21</v>
       </c>
@@ -521,54 +585,54 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E15" s="0" t="n">
-        <f aca="false">CEILING($B$17/H3,1,1)</f>
-        <v>47</v>
-      </c>
-      <c r="F15" s="0" t="n">
-        <f aca="false">CEILING($B$17/G3,1,1)</f>
-        <v>62</v>
-      </c>
-      <c r="G15" s="0" t="n">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="15">
+      <c r="E15" s="0" t="e">
+        <f aca="false">CEILING($B$17/H3,1,1,1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F15" s="0" t="e">
+        <f aca="false">CEILING($B$17/G3,1,1,1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G15" s="0" t="e">
         <f aca="false">E15*C3</f>
-        <v>47</v>
-      </c>
-      <c r="H15" s="0" t="n">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H15" s="0" t="e">
         <f aca="false">F15*D3</f>
-        <v>124</v>
-      </c>
-      <c r="I15" s="0" t="n">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I15" s="0" t="e">
         <f aca="false">AVERAGE(G15:H15)</f>
-        <v>85.5</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="0" t="n">
-        <f aca="false">CEILING($B$17/H4,1,1)</f>
-        <v>21</v>
-      </c>
-      <c r="F16" s="0" t="n">
-        <f aca="false">CEILING($B$17/G4,1,1)</f>
-        <v>31</v>
-      </c>
-      <c r="G16" s="0" t="n">
+      <c r="E16" s="0" t="e">
+        <f aca="false">CEILING($B$17/H4,1,1,1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F16" s="0" t="e">
+        <f aca="false">CEILING($B$17/G4,1,1,1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G16" s="0" t="e">
         <f aca="false">E16*C4</f>
-        <v>42</v>
-      </c>
-      <c r="H16" s="0" t="n">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H16" s="0" t="e">
         <f aca="false">F16*D4</f>
-        <v>93</v>
-      </c>
-      <c r="I16" s="0" t="n">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I16" s="0" t="e">
         <f aca="false">AVERAGE(G16:H16)</f>
-        <v>67.5</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
         <v>20</v>
       </c>
@@ -580,41 +644,41 @@
         <f aca="false">C$22+($B$1-1)*C26</f>
         <v>200</v>
       </c>
-      <c r="E17" s="0" t="n">
-        <f aca="false">CEILING($B$17/H5,1,1)</f>
-        <v>13</v>
-      </c>
-      <c r="F17" s="0" t="n">
-        <f aca="false">CEILING($B$17/G5,1,1)</f>
-        <v>19</v>
-      </c>
-      <c r="G17" s="0" t="n">
+      <c r="E17" s="0" t="e">
+        <f aca="false">CEILING($B$17/H5,1,1,1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F17" s="0" t="e">
+        <f aca="false">CEILING($B$17/G5,1,1,1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G17" s="0" t="e">
         <f aca="false">E17*C5</f>
-        <v>39</v>
-      </c>
-      <c r="H17" s="0" t="n">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H17" s="0" t="e">
         <f aca="false">F17*D5</f>
-        <v>76</v>
-      </c>
-      <c r="I17" s="0" t="n">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I17" s="0" t="e">
         <f aca="false">AVERAGE(G17:H17)</f>
-        <v>57.5</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="0" t="n">
-        <f aca="false">4+FLOOR(($B$1-1)/2,1,1)</f>
-        <v>4</v>
+      <c r="B18" s="0" t="e">
+        <f aca="false">4+FLOOR(($B$1-1)/2,1,1,1)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C18" s="0" t="n">
         <f aca="false">6+($B$1-1)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
         <v>24</v>
       </c>
@@ -625,7 +689,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
         <v>25</v>
       </c>
@@ -636,7 +700,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
         <v>26</v>
       </c>
@@ -647,7 +711,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="24">
       <c r="A24" s="0" t="s">
         <v>27</v>
       </c>
@@ -658,7 +722,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="25">
       <c r="A25" s="0" t="s">
         <v>25</v>
       </c>
@@ -669,7 +733,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
         <v>26</v>
       </c>
@@ -683,10 +747,261 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:O8"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="N11" activeCellId="0" pane="topLeft" sqref="N11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.85"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0051020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9642857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="16.8112244897959"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.6938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="1">
+      <c r="A1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="3">
+      <c r="G3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <f aca="false">FLOOR(B6+(($B$1-1)*$D6)*$B$2,1)</f>
+        <v>69</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <f aca="false">FLOOR(C6+(($B$1-1)*$D6)*$B$2,1)</f>
+        <v>72</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <f aca="false">1+$E6*($B$1-1)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="4">
+      <c r="G4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <f aca="false">FLOOR(B7+(($B$1-1)*$D7)*$B$2,1)</f>
+        <v>58</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <f aca="false">FLOOR(C7+(($B$1-1)*$D7)*$B$2,1)</f>
+        <v>60</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <f aca="false">1+$E7*($B$1-1)</f>
+        <v>10.6</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="5">
+      <c r="A5" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <f aca="false">FLOOR(B8+(($B$1-1)*$D8)*$B$2,1)</f>
+        <v>46</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <f aca="false">FLOOR(C8+(($B$1-1)*$D8)*$B$2,1)</f>
+        <v>47</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <f aca="false">1+$E8*($B$1-1)</f>
+        <v>8.2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="6">
+      <c r="A6" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>1.1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="7">
+      <c r="A7" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="8">
+      <c r="A8" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>1.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>